<commit_message>
full timeline added to draft
</commit_message>
<xml_diff>
--- a/timeline.xlsx
+++ b/timeline.xlsx
@@ -51,6 +51,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -119,7 +120,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -127,7 +128,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -159,16 +160,16 @@
   <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
+      <selection pane="topLeft" activeCell="M6" activeCellId="0" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.52551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.35204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="3.55612244897959"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.5051020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.39795918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="3.51020408163265"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>